<commit_message>
feat(DLR): 3, 4, reorg
</commit_message>
<xml_diff>
--- a/mySyllabus.xlsx
+++ b/mySyllabus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1120" windowWidth="24040" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="24040" windowHeight="14820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
   <si>
     <t>Week</t>
   </si>
@@ -240,24 +240,6 @@
     <t xml:space="preserve"> MLwR C12</t>
   </si>
   <si>
-    <t xml:space="preserve"> HLML 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IDLR 4-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HLML 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IDLR 6-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> HLML 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IDLR 8-9</t>
-  </si>
-  <si>
     <t>IDLR 10-12</t>
   </si>
   <si>
@@ -396,13 +378,25 @@
     <t>Deep Learning with R; Chollet, Allaire</t>
   </si>
   <si>
-    <t>DLR 3-4</t>
-  </si>
-  <si>
-    <t>DLR 5, 7</t>
-  </si>
-  <si>
     <t>DLR 8-9</t>
+  </si>
+  <si>
+    <t>DLR; Hinton</t>
+  </si>
+  <si>
+    <t>DLR 3-5</t>
+  </si>
+  <si>
+    <t>DLR 6-7</t>
+  </si>
+  <si>
+    <t>IDLR 4-5</t>
+  </si>
+  <si>
+    <t>IDLR 6-7</t>
+  </si>
+  <si>
+    <t>IDLR 8-9</t>
   </si>
 </sst>
 </file>
@@ -806,7 +800,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -839,22 +833,22 @@
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>29</v>
@@ -887,7 +881,7 @@
         <v>55</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G2" s="8"/>
       <c r="I2" s="8" t="s">
@@ -920,14 +914,14 @@
         <v>57</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G3" s="8"/>
       <c r="I3" s="9" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>24</v>
@@ -947,14 +941,14 @@
         <v>43149</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G4" s="8"/>
       <c r="I4" s="8" t="s">
         <v>59</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>24</v>
@@ -974,7 +968,7 @@
         <v>43156</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="8" t="s">
@@ -984,7 +978,7 @@
         <v>32</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>12</v>
@@ -1010,7 +1004,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G6" s="8"/>
       <c r="I6" s="8" t="s">
@@ -1020,7 +1014,7 @@
         <v>33</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1040,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1080,7 +1074,7 @@
         <v>61</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>62</v>
@@ -1095,7 +1089,7 @@
         <v>35</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>14</v>
@@ -1103,7 +1097,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="2"/>
@@ -1133,20 +1127,17 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="G10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>24</v>
+      <c r="L10" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>8</v>
@@ -1166,22 +1157,19 @@
         <v>43198</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="J11" s="1" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>37</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1201,20 +1189,17 @@
         <v>6</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="J12" s="1" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>38</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>14</v>
@@ -1240,7 +1225,7 @@
         <v>69</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>39</v>
@@ -1295,7 +1280,7 @@
         <v>41</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>17</v>
@@ -1321,7 +1306,7 @@
         <v>42</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>10</v>
@@ -1365,13 +1350,13 @@
     </row>
     <row r="21" spans="1:14">
       <c r="L21" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1404,7 +1389,7 @@
         <v>45</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1429,13 +1414,13 @@
         <v>25</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>45</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1446,32 +1431,32 @@
         <v>28</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="L28" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1493,67 +1478,68 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="L35" s="10"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="11" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
feat(CNN):  DLR prep and Imagenet transfer methods
</commit_message>
<xml_diff>
--- a/mySyllabus.xlsx
+++ b/mySyllabus.xlsx
@@ -800,7 +800,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1162,7 +1162,7 @@
       <c r="H11" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K11" s="2" t="s">

</xml_diff>

<commit_message>
feat(dataprep): validation reorg scripts
</commit_message>
<xml_diff>
--- a/mySyllabus.xlsx
+++ b/mySyllabus.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Syllabus" sheetId="1" r:id="rId1"/>
-    <sheet name="FinalPaperNotes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="119">
   <si>
     <t>Week</t>
   </si>
@@ -181,18 +180,6 @@
   </si>
   <si>
     <t>https://towardsdatascience.com/the-8-neural-network-architectures-machine-learning-researchers-need-to-learn-11a0c96d6073</t>
-  </si>
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why do we need Deep Learning?   What challenges is it good for </t>
-  </si>
-  <si>
-    <t>DL 5.11</t>
   </si>
   <si>
     <t>MYNN P1</t>
@@ -803,7 +790,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -836,22 +823,22 @@
         <v>5</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>29</v>
@@ -881,14 +868,14 @@
         <v>6</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G2" s="8"/>
       <c r="I2" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>31</v>
@@ -914,17 +901,17 @@
         <v>6</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G3" s="8"/>
       <c r="I3" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L3" s="8" t="s">
         <v>24</v>
@@ -944,14 +931,14 @@
         <v>43149</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L4" s="8" t="s">
         <v>24</v>
@@ -971,17 +958,17 @@
         <v>43156</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K5" s="8" t="s">
         <v>32</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>12</v>
@@ -1007,17 +994,17 @@
         <v>6</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G6" s="8"/>
       <c r="I6" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1037,15 +1024,15 @@
         <v>6</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>34</v>
@@ -1074,25 +1061,25 @@
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>14</v>
@@ -1100,7 +1087,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="2"/>
@@ -1131,16 +1118,16 @@
         <v>6</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>36</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>8</v>
@@ -1160,19 +1147,19 @@
         <v>43198</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>37</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1191,18 +1178,19 @@
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="J12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="G12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>114</v>
+      <c r="L12" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>14</v>
@@ -1225,10 +1213,10 @@
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>39</v>
@@ -1283,7 +1271,7 @@
         <v>41</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="M15" s="1" t="s">
         <v>17</v>
@@ -1309,7 +1297,7 @@
         <v>42</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>10</v>
@@ -1352,17 +1340,15 @@
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="H21" s="13">
-        <v>13000000000</v>
-      </c>
+      <c r="H21" s="13"/>
       <c r="L21" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1395,7 +1381,7 @@
         <v>45</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1420,13 +1406,13 @@
         <v>25</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="M25" s="1" t="s">
         <v>45</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1437,32 +1423,32 @@
         <v>28</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:14">
       <c r="L28" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1484,101 +1470,67 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="L35" s="10"/>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="11" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>